<commit_message>
updated Rservice listing excel
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVWDemo_RServiceListing.xlsx
+++ b/docs/OVW Sheets/OVWDemo_RServiceListing.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVW Migration Dec 29\OVWMigration\docs\OVW Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVW-jan8\OVWMigration\docs\OVW Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19410" windowHeight="9735" firstSheet="15" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19410" windowHeight="9735" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="ar_ae" sheetId="25" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="167">
   <si>
     <t>http://www.cisco.com/web/ANZ/products/routers/services.html</t>
   </si>
@@ -559,6 +559,12 @@
   </si>
   <si>
     <t>http://www.cisco.com/web/CA/products/wireless/services_fr.html</t>
+  </si>
+  <si>
+    <t>service-listing-Rvar2</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DE/products/unified_computing/services.html</t>
   </si>
 </sst>
 </file>
@@ -930,7 +936,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,6 +995,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -1010,7 +1019,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,6 +1078,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -1091,7 +1103,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,6 +1162,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -1172,7 +1187,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,6 +1246,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -1251,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,6 +1329,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -1332,7 +1353,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1391,6 +1412,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -1412,7 +1436,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,6 +1495,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -1491,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,6 +1578,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -1572,7 +1602,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1631,6 +1661,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -1652,7 +1685,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1711,7 +1744,9 @@
       <c r="B4" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1733,7 +1768,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1792,6 +1827,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -1813,7 +1851,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1872,7 +1910,9 @@
       <c r="B4" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1894,7 +1934,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1953,6 +1993,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -1974,7 +2017,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,6 +2076,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -2054,7 +2100,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2113,6 +2159,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -2134,7 +2183,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2193,6 +2242,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -2214,7 +2266,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,6 +2325,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -2293,8 +2348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2353,6 +2408,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -2374,7 +2432,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2433,6 +2491,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -2454,7 +2515,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2513,6 +2574,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -2534,13 +2598,13 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="72.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2572,7 +2636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>102</v>
       </c>
@@ -2592,6 +2656,9 @@
       </c>
       <c r="B4" t="s">
         <v>122</v>
+      </c>
+      <c r="C4" t="s">
+        <v>165</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -2614,7 +2681,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2673,6 +2740,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -2694,7 +2764,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2753,7 +2823,9 @@
       <c r="B4" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
@@ -2775,7 +2847,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2834,6 +2906,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -2854,8 +2929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2914,6 +2989,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -2935,7 +3013,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2994,6 +3072,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -3015,7 +3096,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3074,6 +3155,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -3095,7 +3179,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3154,6 +3238,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -3174,8 +3261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3234,6 +3321,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -3254,8 +3344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3314,6 +3404,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -3335,7 +3428,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3394,6 +3487,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -3415,7 +3511,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3474,6 +3570,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -3495,7 +3594,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3554,6 +3653,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -3572,10 +3674,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3627,11 +3729,27 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="B4" r:id="rId5" display="http://www.cisco.com/c/en/us/products/servers-unified-computing/service-listing.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3642,7 +3760,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3701,6 +3819,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -3722,7 +3843,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3757,7 +3878,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3816,7 +3937,9 @@
       <c r="B4" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
@@ -3838,7 +3961,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3897,6 +4020,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -3918,7 +4044,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3977,7 +4103,9 @@
       <c r="B4" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
@@ -3999,7 +4127,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4058,7 +4186,9 @@
       <c r="B4" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
@@ -4080,7 +4210,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4139,6 +4269,9 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>

</xml_diff>